<commit_message>
Minor bugs and GPIO unknown state fixes
Change log:
- Updated CELL net Connection (pin 2 MAX17043)
-Removed solder jumpers for IMU
-Added pull up resistors for SDA and SCL on IMU
-Updated power net for Aux switches from VIN to 3V3
-Removed Shutdown LED circuitry (too complex for current design
parameters)
-Updated Sleeve net connection on 3.5mm jack

Outstanding/Research:
-Pull up resistor on AD5220 CLK (see schematic for proposed fix)
</commit_message>
<xml_diff>
--- a/Photon_Dev/Time Sheet/Timesheet.xlsx
+++ b/Photon_Dev/Time Sheet/Timesheet.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Madison\Desktop\Photon_Dev\Time Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Madison\Desktop\gc\Photon_Dev\Time Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="10-12-15 to 10-23-15" sheetId="1" r:id="rId1"/>
+    <sheet name="10-24-15 to 11-04-15" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -54,6 +55,24 @@
   </si>
   <si>
     <t>Control bus and signal wiring. Modified the digital pot choice to fit pin requirements</t>
+  </si>
+  <si>
+    <t>Started Footprint creation for P1 and other IC's</t>
+  </si>
+  <si>
+    <t>Pad design for most footprints</t>
+  </si>
+  <si>
+    <t>Initial Footprint creation completed/ Design Rules Check</t>
+  </si>
+  <si>
+    <t>Connector Placement on PCB. Set up design rules for placement</t>
+  </si>
+  <si>
+    <t>Audio, Power, Charger Circuitry placed on PCB. Updated connector placement</t>
+  </si>
+  <si>
+    <t>Fixed outstanding schematic issues from intial review</t>
   </si>
 </sst>
 </file>
@@ -99,14 +118,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,10 +431,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>42289</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2">
@@ -423,10 +442,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>42290</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3">
@@ -434,10 +453,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>42292</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4">
@@ -445,10 +464,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>42294</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -456,10 +475,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>42296</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6">
@@ -467,10 +486,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>42298</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7">
@@ -478,10 +497,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="3"/>
       <c r="C16">
         <f>SUM(C2:C7)</f>
         <v>5.5</v>
@@ -494,4 +513,113 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>42301</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>42303</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>42307</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>42309</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>42311</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>42312</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16">
+        <f>SUM(C2:C7)</f>
+        <v>6.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
External IMU Board added
- Updated artwork (Sleeptrack V2 Final)
-Created IMU External PCB and Schematic
</commit_message>
<xml_diff>
--- a/Photon_Dev/Time Sheet/Timesheet.xlsx
+++ b/Photon_Dev/Time Sheet/Timesheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="10-12-15 to 10-23-15" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="11-05-15 to 11-17-15" sheetId="3" r:id="rId3"/>
     <sheet name="11-18-15 to 12-17-15" sheetId="4" r:id="rId4"/>
     <sheet name="12-18-15 to 02-02-16" sheetId="5" r:id="rId5"/>
+    <sheet name="02-03-16_to_02-28-16" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -139,6 +140,21 @@
   </si>
   <si>
     <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>Completed V2 update. 1:1 Artwork Check, verify components, etc.</t>
+  </si>
+  <si>
+    <t>Research small run board houses. Submit Files for manufacture/assembly quote to American Circuits, Circuitology, Screaming Circuits</t>
+  </si>
+  <si>
+    <t>Updated SleepTrack PCB  to V2</t>
+  </si>
+  <si>
+    <t>Sent Components to elecrow</t>
+  </si>
+  <si>
+    <t>Start Layout for remote IMU board</t>
   </si>
 </sst>
 </file>
@@ -182,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -211,10 +227,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +604,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="13"/>
       <c r="C16">
         <f>SUM(C2:C7)</f>
         <v>5.5</v>
@@ -695,10 +714,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="13"/>
       <c r="C16">
         <f>SUM(C2:C7)</f>
         <v>6.25</v>
@@ -1019,14 +1038,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1041,7 +1060,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>42356</v>
       </c>
       <c r="B2" t="s">
@@ -1052,7 +1071,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>42360</v>
       </c>
       <c r="B3" t="s">
@@ -1063,7 +1082,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>42360</v>
       </c>
       <c r="B4" t="s">
@@ -1074,7 +1093,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>42380</v>
       </c>
       <c r="B5" t="s">
@@ -1085,7 +1104,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>42395</v>
       </c>
       <c r="B6" t="s">
@@ -1096,7 +1115,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="12"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1110,4 +1129,105 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>42407</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>42411</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>42412</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>42423</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>42428</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f>SUM(C2:C6)</f>
+        <v>5.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>